<commit_message>
Add revenue in output of parent utpr calcs
</commit_message>
<xml_diff>
--- a/outputs/oecd_puerto_rico_totals_by_year_profit_positive.xlsx
+++ b/outputs/oecd_puerto_rico_totals_by_year_profit_positive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Documents/GitHub/Repos/Espacios-Abiertos/recolecta-corporaciones/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A0C346-5BEF-8E40-9CFB-7C7005AE4B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC4279C-E6DD-C145-BC9B-34A93ED483D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8611A138-D958-554C-B58D-0523D03C5B92}"/>
   </bookViews>
@@ -243,7 +243,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,###.#,,&quot;M&quot;"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.0,,&quot;M&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0,,&quot;M&quot;"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -751,7 +751,7 @@
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1129,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F403C0-4FDC-D847-95D8-3FE58FEE280F}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
so many presentation table stuff
</commit_message>
<xml_diff>
--- a/outputs/oecd_puerto_rico_totals_by_year_profit_positive.xlsx
+++ b/outputs/oecd_puerto_rico_totals_by_year_profit_positive.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10728"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabriel/Documents/GitHub/Repos/Espacios-Abiertos/recolecta-corporaciones/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC4279C-E6DD-C145-BC9B-34A93ED483D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43811D94-7E68-A84E-B604-052E558C8C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{8611A138-D958-554C-B58D-0523D03C5B92}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>time_period</t>
   </si>
@@ -129,21 +129,12 @@
     <t>Income tax accrued - current year</t>
   </si>
   <si>
-    <t>Impuestos</t>
-  </si>
-  <si>
     <t>Employees</t>
   </si>
   <si>
-    <t>Empleos</t>
-  </si>
-  <si>
     <t>Entities</t>
   </si>
   <si>
-    <t>Subsidiarias</t>
-  </si>
-  <si>
     <t>Tangible assets other than cash and cash equivalents</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>Substance based income exclusion</t>
   </si>
   <si>
-    <t>Inclusión de ingresos basado en la sustancia</t>
-  </si>
-  <si>
     <t>Excess profit</t>
   </si>
   <si>
@@ -235,17 +223,33 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>Impuestos devengados</t>
+  </si>
+  <si>
+    <t>Número de empleados</t>
+  </si>
+  <si>
+    <t>Número de corporaciones foráneas</t>
+  </si>
+  <si>
+    <t>Exclusión de ingresos basada en la sustancia</t>
+  </si>
+  <si>
+    <t>Variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,###.#,,&quot;M&quot;"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.0,,&quot;M&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,###.0,,&quot;M&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,8 +399,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Bernino Sans"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Bernino Sans"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +591,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF707DC8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -737,13 +760,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -751,7 +771,16 @@
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -799,6 +828,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF707DC8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1129,578 +1163,597 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F403C0-4FDC-D847-95D8-3FE58FEE280F}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="2" cm="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.3">
+      <c r="C1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="8" cm="1">
         <f t="array" ref="D1:I1">TRANSPOSE(totals_profit_positive!A2:A7)</f>
         <v>2016</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="8">
         <v>2017</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="8">
         <v>2018</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="8">
         <v>2019</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="8">
         <v>2020</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="8">
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A2" t="str" cm="1">
         <f t="array" ref="A2:A15">TRANSPOSE(totals_profit_positive!B1:O1)</f>
         <v>TOT_REV</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="9" t="str">
         <f>_xlfn.XLOOKUP(A2,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Total revenues</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="9" t="str">
         <f>_xlfn.XLOOKUP(A2,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Ingresos totales</v>
       </c>
-      <c r="D2" s="3" cm="1">
+      <c r="D2" s="10" cm="1">
         <f t="array" ref="D2:I15">TRANSPOSE(totals_profit_positive!B2:O7)</f>
         <v>96666285550.815002</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>93649941007</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="10">
         <v>116690866514.95599</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="10">
         <v>99391737988</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="10">
         <v>96447665894.800003</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="10">
         <v>105065023711</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <v>PROFIT</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="9" t="str">
         <f>_xlfn.XLOOKUP(A3,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Profit (loss) before income tax</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="9" t="str">
         <f>_xlfn.XLOOKUP(A3,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Beneficios</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="10">
         <v>39192043678.124001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="10">
         <v>35777656315</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="10">
         <v>38999967418.857002</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="10">
         <v>35477255086.5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="10">
         <v>37412603822.934998</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="10">
         <v>32927750696</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <v>TAX_ACCRUED</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="9" t="str">
         <f>_xlfn.XLOOKUP(A4,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Income tax accrued - current year</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="9" t="str">
         <f>_xlfn.XLOOKUP(A4,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
-        <v>Impuestos</v>
-      </c>
-      <c r="D4" s="3">
+        <v>Impuestos devengados</v>
+      </c>
+      <c r="D4" s="10">
         <v>393363924.29799998</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="10">
         <v>526139986.00999999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>1230550961.0899999</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="10">
         <v>512820083.90999901</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="10">
         <v>582624717.72099996</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="10">
         <v>798824190</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <v>EMPLOYEES</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="9" t="str">
         <f>_xlfn.XLOOKUP(A5,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Employees</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="9" t="str">
         <f>_xlfn.XLOOKUP(A5,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
-        <v>Empleos</v>
-      </c>
-      <c r="D5" s="4">
+        <v>Número de empleados</v>
+      </c>
+      <c r="D5" s="11">
         <v>58777</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="11">
         <v>57029</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="11">
         <v>66700</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="11">
         <v>70056</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="11">
         <v>73777.733999999997</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="11">
         <v>88510</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <v>ENTITIES_COUNT</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="9" t="str">
         <f>_xlfn.XLOOKUP(A6,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Entities</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="9" t="str">
         <f>_xlfn.XLOOKUP(A6,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
-        <v>Subsidiarias</v>
-      </c>
-      <c r="D6" s="4">
+        <v>Número de corporaciones foráneas</v>
+      </c>
+      <c r="D6" s="11">
         <v>2</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="11">
         <v>146</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="11">
         <v>141</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="11">
         <v>89</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="11">
         <v>94</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="11">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <v>ASSETS</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="9" t="str">
         <f>_xlfn.XLOOKUP(A7,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Tangible assets other than cash and cash equivalents</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="9" t="str">
         <f>_xlfn.XLOOKUP(A7,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Activos tangibles</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="15">
         <v>15994019880.475</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="15">
         <v>15331260643.4</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="15">
         <v>27062914820.646999</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="15">
         <v>18119955517.799999</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="15">
         <v>17441096461.580002</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="15">
         <v>23997321263</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <v>EARNINGS</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="9" t="str">
         <f>_xlfn.XLOOKUP(A8,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Accumulated earnings</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="9" t="str">
         <f>_xlfn.XLOOKUP(A8,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Ganancias acumuladas</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="15">
         <v>100056189106.203</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="15">
         <v>114313493903.56</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="15">
         <v>24297798981.507</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="15">
         <v>39572004893.599998</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="15">
         <v>33970552286.330002</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="15">
         <v>19530873629</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <v>PAYROLL</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="9" t="str">
         <f>_xlfn.XLOOKUP(A9,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Payroll</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="9" t="str">
         <f>_xlfn.XLOOKUP(A9,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Nómina</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="10">
         <v>2459256717.4199901</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="10">
         <v>2386119593.3400002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="10">
         <v>2790758682</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="10">
         <v>2931175265.7599902</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="10">
         <v>3086894328.3176398</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="10">
         <v>3703299114.5999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <v>TAX_BASE</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="9" t="str">
         <f>_xlfn.XLOOKUP(A10,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Tax base</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="9" t="str">
         <f>_xlfn.XLOOKUP(A10,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Base tributaria</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="10">
         <v>37666596415.944</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="10">
         <v>34241307288.914001</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="10">
         <v>36555858365.005203</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="10">
         <v>33734541118.499901</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="10">
         <v>35708626673.176804</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="10">
         <v>30637635083.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <v>SBIE</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="9" t="str">
         <f>_xlfn.XLOOKUP(A11,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Substance based income exclusion</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="9" t="str">
         <f>_xlfn.XLOOKUP(A11,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
-        <v>Inclusión de ingresos basado en la sustancia</v>
-      </c>
-      <c r="D11" s="3">
+        <v>Exclusión de ingresos basada en la sustancia</v>
+      </c>
+      <c r="D11" s="10">
         <v>1525447262.1799901</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="10">
         <v>1458329974.086</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="10">
         <v>2444109053.8517599</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="10">
         <v>1742713968</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="10">
         <v>1703977149.7581601</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="10">
         <v>2290115612.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <v>EXCESS_PROFIT</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="9" t="str">
         <f>_xlfn.XLOOKUP(A12,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Excess profit</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="9" t="str">
         <f>_xlfn.XLOOKUP(A12,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Beneficio excedente</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="10">
         <v>95140838288.634995</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="10">
         <v>91844702490.914001</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="10">
         <v>114246757461.104</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="10">
         <v>97649024020</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="10">
         <v>94743688745.041794</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="10">
         <v>102774908098.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <v>ETR</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="9" t="str">
         <f>_xlfn.XLOOKUP(A13,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Effective Tax Rate</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="9" t="str">
         <f>_xlfn.XLOOKUP(A13,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Tasa efectiva contributiva</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="12">
         <v>1.00368311366616E-2</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="12">
         <v>1.47058259316279E-2</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="12">
         <v>3.1552615105391403E-2</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="12">
         <v>1.4454897445127899E-2</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="12">
         <v>1.5572952913900999E-2</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="12">
         <v>2.42599076194123E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <v>TTR</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="9" t="str">
         <f>_xlfn.XLOOKUP(A14,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Top-up tax rate</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="9" t="str">
         <f>_xlfn.XLOOKUP(A14,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Impuesto complementario</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="12">
         <v>0.13996316886333801</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="12">
         <v>0.13529417406837199</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="12">
         <v>0.118447384894608</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="12">
         <v>0.13554510255487201</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="12">
         <v>0.13442704708609801</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="12">
         <v>0.125740092380587</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="19" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <v>QDMTT</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="9" t="str">
         <f>_xlfn.XLOOKUP(A15,cbc_labels!$A$2:$A$16,cbc_labels!$B$2:$B$16)</f>
         <v>Qualifying domestic minimum top-up tax</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="9" t="str">
         <f>_xlfn.XLOOKUP(A15,cbc_labels!$A$2:$A$16,cbc_labels!$C$2:$C$16)</f>
         <v>Impuesto complementario mínimo nacional calificado</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="10">
         <v>5271936194.6719799</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="10">
         <v>4632649388.6749401</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="10">
         <v>4329945825.91257</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="10">
         <v>4572551835.5486298</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="10">
         <v>4800205239.1750698</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="10">
         <v>3852379065.7220201</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="11" cm="1">
+      <c r="C18" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="14" cm="1">
         <f t="array" ref="D18:I18">_xlfn.ANCHORARRAY(iir_profit_positive!F2)</f>
         <v>5271717108.3920002</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="14">
         <v>4591735139.974</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="14">
         <v>4314324046.9119997</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="14">
         <v>4488609144.0880003</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="14">
         <v>4659717023.8979998</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="14">
         <v>3774018117.7150002</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="11" cm="1">
+    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="14" cm="1">
         <f t="array" ref="D19:I19">_xlfn.ANCHORARRAY(iir_profit_positive!F3)</f>
         <v>13548.763999999999</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="14">
         <v>30386273.225000001</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="14">
         <v>17311200.851</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G19" s="14">
         <v>58184933.327</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="14">
         <v>118765956.169</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="14">
         <v>60723875.048</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="11" cm="1">
+    <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="14" cm="1">
         <f t="array" ref="D20:I20">_xlfn.ANCHORARRAY(iir_profit_positive!F4)</f>
         <v>205537.51699999999</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="14">
         <v>10527975.476</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="14">
         <v>-1689421.85</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="14">
         <v>25757758.134</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="14">
         <v>21722259.107999999</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="14">
         <v>17637072.958999999</v>
       </c>
     </row>
@@ -2072,14 +2125,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>46</v>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F1" cm="1">
         <f t="array" ref="F1:K1">TRANSPOSE(B2:B7)</f>
@@ -2102,17 +2155,17 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="6">
         <v>2016</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="7">
         <v>5271717108.3920002</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F2" cm="1">
         <f t="array" ref="F2:K2">TRANSPOSE(C2:C7)</f>
@@ -2135,17 +2188,17 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6">
         <v>2017</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>4591735139.974</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F3" cm="1">
         <f t="array" ref="F3:K3">TRANSPOSE(C8:C13)</f>
@@ -2168,17 +2221,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="6">
         <v>2018</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <v>4314324046.9119997</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4:K4">TRANSPOSE(C14:C19)</f>
@@ -2201,167 +2254,167 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="6">
         <v>2019</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <v>4488609144.0880003</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="6">
         <v>2020</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>4659717023.8979998</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="9">
+      <c r="A7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="6">
         <v>2021</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="7">
         <v>3774018117.7150002</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="9">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="6">
         <v>2016</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>13548.763999999999</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="9">
+      <c r="A9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="6">
         <v>2017</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <v>30386273.225000001</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="6">
         <v>2018</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>17311200.851</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="6">
         <v>2019</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>58184933.327</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6">
         <v>2020</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>118765956.169</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="9">
+      <c r="A13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6">
         <v>2021</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <v>60723875.048</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="9">
+      <c r="A14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="6">
         <v>2016</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <v>205537.51699999999</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="A15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="6">
         <v>2017</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>10527975.476</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="9">
+      <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="6">
         <v>2018</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>-1689421.85</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="9">
+      <c r="A17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="6">
         <v>2019</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="7">
         <v>25757758.134</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="9">
+      <c r="A18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6">
         <v>2020</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>21722259.107999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="9">
+      <c r="A19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="6">
         <v>2021</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>17637072.958999999</v>
       </c>
     </row>
@@ -2374,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E200D4-A4F5-D24D-9312-DF8A090B9112}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:C16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,179 +2439,179 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="7" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="C12" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C13" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>